<commit_message>
Überprüfung UML Diagramme für Prototyp 6
Testprotokolle für die UML Diagramme erstellt.
Die Überprüfung der Klassendiagramme wurde noch nicht erledigt da diese
noch auf den Prototyp Version 6 angepasst werden müssen.
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="Auswahl">'Aufgaben_Alle ( Axx )'!$AJ$4:$AJ$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$60</definedName>
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="58">
   <si>
     <t>SWE Projekt HFTL-APP</t>
   </si>
@@ -377,7 +377,175 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -748,9 +916,9 @@
   <dimension ref="A1:BE399"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
+      <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="18.75" customHeight="1"/>
@@ -759,7 +927,7 @@
     <col min="2" max="2" width="7.109375" style="11" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="11" customWidth="1"/>
     <col min="4" max="5" width="14.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="17.109375" style="11" customWidth="1"/>
     <col min="9" max="9" width="17.109375" style="10" customWidth="1"/>
     <col min="10" max="10" width="17.109375" style="8" customWidth="1"/>
@@ -2243,108 +2411,252 @@
       </c>
     </row>
     <row r="49" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B49" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="B49" s="16">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C49" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I49" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J49" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B50" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="B50" s="16">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C50" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I50" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J50" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="51" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B51" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="B51" s="16">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C51" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I51" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J51" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="52" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B52" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
+      <c r="B52" s="16">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C52" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I52" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J52" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="53" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B53" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
+      <c r="B53" s="16">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C53" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I53" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J53" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B54" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
+      <c r="B54" s="16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C54" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I54" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J54" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B55" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
+      <c r="B55" s="16">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C55" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I55" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J55" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="56" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B56" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
+      <c r="B56" s="16">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C56" s="9">
+        <v>42236</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I56" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J56" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="57" spans="2:10" ht="18.75" customHeight="1">
       <c r="B57" s="16" t="str">
@@ -5304,13 +5616,13 @@
     <sortCondition ref="BE16"/>
   </sortState>
   <conditionalFormatting sqref="B5:J1048576">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="32" priority="7">
       <formula>$J5="bestanden"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>OR($I5="ungenügend",$I5="mangelhaft")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="30" priority="9">
       <formula>$B5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Tests durchgeführt, Dokumentation weiter bearbeitet
4.6.4 Nummerierung falsch? Anpassen!!!!!  Erledigt!!
Softwaretests nicht alle?

4.3.3 APP Layout eingefügt

4.3.4 löschen? !!!!!!!!!!!!!!!!  Gelöscht!

4.7.3 Projektstukturplan? Welcher? Ist das nicht der aus 4.7.2?  Noch in
Klärung

4.7.4 Release-History eingefügt, kann das so bleiben? Dort sollen die
Releases bleiben

4.7.5 Testbogen eingefügt ---- Testbögen von allen modulen in den
Anhang, Testprotokoll mit ID einfügen

4.5.3 das gleiche wie 4.7.4?   ( wird noch geklärt )

UML einfach in den Anhang

Sollte das Entwicklerhandbuch nicht mit in den Anhang?  Erst wenn Stefan
fertig ist

Wie sollen die ganzen Sitzungs/TestProtokolle angefügt werden?  Tests
bis 24.08 eingefügt

Entwicklerhandbuch in Anhang eingefügt  Leider nur mit subsubsubsection
Evtl.als externe  PDF einbinden
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben_Alle ( Axx )" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="58">
   <si>
     <t>SWE Projekt HFTL-APP</t>
   </si>
@@ -200,8 +200,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,217 +377,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -629,9 +419,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -669,9 +459,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,9 +493,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -737,9 +528,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -912,32 +704,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE399"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="11" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="1.6640625" style="1" customWidth="1"/>
-    <col min="12" max="55" width="14.33203125" style="1"/>
-    <col min="56" max="56" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="14.33203125" style="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="11" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="1" customWidth="1"/>
+    <col min="12" max="55" width="14.28515625" style="1"/>
+    <col min="56" max="56" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="14.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="18.75" hidden="1" customHeight="1">
+    <row r="1" spans="1:57" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -951,7 +743,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:57" ht="18.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:57" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="18.75" customHeight="1">
+    <row r="3" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="1"/>
@@ -978,7 +770,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:57" ht="18.75" customHeight="1">
+    <row r="4" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>22</v>
       </c>
@@ -1007,7 +799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="28.8">
+    <row r="5" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>1</v>
       </c>
@@ -1037,7 +829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="28.8">
+    <row r="6" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <f>IF(C6="","",B5+1)</f>
         <v>2</v>
@@ -1068,7 +860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="28.8">
+    <row r="7" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <f t="shared" ref="B7:B72" si="0">IF(C7="","",B6+1)</f>
         <v>3</v>
@@ -1099,7 +891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="28.8">
+    <row r="8" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1135,7 +927,7 @@
       <c r="BD8" s="17"/>
       <c r="BE8" s="8"/>
     </row>
-    <row r="9" spans="1:57" ht="14.4">
+    <row r="9" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1184,7 +976,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="18.75" customHeight="1">
+    <row r="10" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1233,7 +1025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="14.4">
+    <row r="11" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1279,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="18.75" customHeight="1">
+    <row r="12" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1325,7 +1117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="14.4">
+    <row r="13" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1369,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="14.4">
+    <row r="14" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1412,7 +1204,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="14.4">
+    <row r="15" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1446,7 +1238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:57" ht="14.4">
+    <row r="16" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1480,7 +1272,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="28.8">
+    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1511,7 +1303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="14.4">
+    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1536,7 +1328,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="2:10" ht="18.75" customHeight="1">
+    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1567,7 +1359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="18.75" customHeight="1">
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1598,7 +1390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="18.75" customHeight="1">
+    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1629,7 +1421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="28.8">
+    <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1650,7 +1442,7 @@
       <c r="H22" s="9"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="2:10" ht="18.75" customHeight="1">
+    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1671,7 +1463,7 @@
       <c r="H23" s="9"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="2:10" ht="18.75" customHeight="1">
+    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1702,7 +1494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="18.75" customHeight="1">
+    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1733,7 +1525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="18.75" customHeight="1">
+    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1764,7 +1556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="18.75" customHeight="1">
+    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1795,7 +1587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="18.75" customHeight="1">
+    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1826,7 +1618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="18.75" customHeight="1">
+    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1857,7 +1649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="18.75" customHeight="1">
+    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1882,7 +1674,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="2:10" ht="18.75" customHeight="1">
+    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="16">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1907,7 +1699,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="2:10" ht="18.75" customHeight="1">
+    <row r="32" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="16">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1932,7 +1724,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="2:10" ht="18.75" customHeight="1">
+    <row r="33" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="16">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1963,7 +1755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="18.75" customHeight="1">
+    <row r="34" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1994,7 +1786,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="18.75" customHeight="1">
+    <row r="35" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="16">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2025,7 +1817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="18.75" customHeight="1">
+    <row r="36" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="16">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2056,7 +1848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="18.75" customHeight="1">
+    <row r="37" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="16">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2087,7 +1879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="18.75" customHeight="1">
+    <row r="38" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="16">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2118,7 +1910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="18.75" customHeight="1">
+    <row r="39" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="16">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2149,7 +1941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="18.75" customHeight="1">
+    <row r="40" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="16">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2180,7 +1972,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="18.75" customHeight="1">
+    <row r="41" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="16">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2211,7 +2003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="18.75" customHeight="1">
+    <row r="42" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="16">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2242,7 +2034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="18.75" customHeight="1">
+    <row r="43" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="16">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2259,15 +2051,21 @@
       <c r="F43" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I43" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="2:10" ht="18.75" customHeight="1">
+        <v>sehr gut</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="16">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2284,15 +2082,21 @@
       <c r="F44" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="G44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I44" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="2:10" ht="18.75" customHeight="1">
+        <v>gut</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="16">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2309,15 +2113,21 @@
       <c r="F45" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="G45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I45" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J45" s="9"/>
-    </row>
-    <row r="46" spans="2:10" ht="18.75" customHeight="1">
+        <v>sehr gut</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2348,7 +2158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:10" ht="18.75" customHeight="1">
+    <row r="47" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="16">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2379,7 +2189,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="18.75" customHeight="1">
+    <row r="48" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2410,7 +2220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="18.75" customHeight="1">
+    <row r="49" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="16">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2441,7 +2251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="18.75" customHeight="1">
+    <row r="50" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="16">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2472,7 +2282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="18.75" customHeight="1">
+    <row r="51" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="16">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2503,7 +2313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="18.75" customHeight="1">
+    <row r="52" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="16">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2534,7 +2344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="18.75" customHeight="1">
+    <row r="53" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2565,7 +2375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="18.75" customHeight="1">
+    <row r="54" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="16">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2596,7 +2406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="18.75" customHeight="1">
+    <row r="55" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="16">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2627,7 +2437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="18.75" customHeight="1">
+    <row r="56" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="16">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2658,7 +2468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="2:10" ht="18.75" customHeight="1">
+    <row r="57" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2671,7 +2481,7 @@
       </c>
       <c r="J57" s="9"/>
     </row>
-    <row r="58" spans="2:10" ht="18.75" customHeight="1">
+    <row r="58" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2684,7 +2494,7 @@
       </c>
       <c r="J58" s="9"/>
     </row>
-    <row r="59" spans="2:10" ht="18.75" customHeight="1">
+    <row r="59" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2697,7 +2507,7 @@
       </c>
       <c r="J59" s="9"/>
     </row>
-    <row r="60" spans="2:10" ht="18.75" customHeight="1">
+    <row r="60" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2710,7 +2520,7 @@
       </c>
       <c r="J60" s="9"/>
     </row>
-    <row r="61" spans="2:10" ht="18.75" customHeight="1">
+    <row r="61" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2723,7 +2533,7 @@
       </c>
       <c r="J61" s="9"/>
     </row>
-    <row r="62" spans="2:10" ht="18.75" customHeight="1">
+    <row r="62" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2736,7 +2546,7 @@
       </c>
       <c r="J62" s="9"/>
     </row>
-    <row r="63" spans="2:10" ht="18.75" customHeight="1">
+    <row r="63" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2749,7 +2559,7 @@
       </c>
       <c r="J63" s="9"/>
     </row>
-    <row r="64" spans="2:10" ht="18.75" customHeight="1">
+    <row r="64" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2762,7 +2572,7 @@
       </c>
       <c r="J64" s="9"/>
     </row>
-    <row r="65" spans="2:10" ht="18.75" customHeight="1">
+    <row r="65" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2775,7 +2585,7 @@
       </c>
       <c r="J65" s="9"/>
     </row>
-    <row r="66" spans="2:10" ht="18.75" customHeight="1">
+    <row r="66" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2788,7 +2598,7 @@
       </c>
       <c r="J66" s="9"/>
     </row>
-    <row r="67" spans="2:10" ht="18.75" customHeight="1">
+    <row r="67" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2801,7 +2611,7 @@
       </c>
       <c r="J67" s="9"/>
     </row>
-    <row r="68" spans="2:10" ht="18.75" customHeight="1">
+    <row r="68" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2814,7 +2624,7 @@
       </c>
       <c r="J68" s="9"/>
     </row>
-    <row r="69" spans="2:10" ht="18.75" customHeight="1">
+    <row r="69" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2827,7 +2637,7 @@
       </c>
       <c r="J69" s="9"/>
     </row>
-    <row r="70" spans="2:10" ht="18.75" customHeight="1">
+    <row r="70" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2840,7 +2650,7 @@
       </c>
       <c r="J70" s="9"/>
     </row>
-    <row r="71" spans="2:10" ht="18.75" customHeight="1">
+    <row r="71" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2853,7 +2663,7 @@
       </c>
       <c r="J71" s="9"/>
     </row>
-    <row r="72" spans="2:10" ht="18.75" customHeight="1">
+    <row r="72" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2866,7 +2676,7 @@
       </c>
       <c r="J72" s="9"/>
     </row>
-    <row r="73" spans="2:10" ht="18.75" customHeight="1">
+    <row r="73" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="str">
         <f t="shared" ref="B73:B136" si="2">IF(C73="","",B72+1)</f>
         <v/>
@@ -2879,7 +2689,7 @@
       </c>
       <c r="J73" s="9"/>
     </row>
-    <row r="74" spans="2:10" ht="18.75" customHeight="1">
+    <row r="74" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2892,7 +2702,7 @@
       </c>
       <c r="J74" s="9"/>
     </row>
-    <row r="75" spans="2:10" ht="18.75" customHeight="1">
+    <row r="75" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2905,7 +2715,7 @@
       </c>
       <c r="J75" s="9"/>
     </row>
-    <row r="76" spans="2:10" ht="18.75" customHeight="1">
+    <row r="76" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2918,7 +2728,7 @@
       </c>
       <c r="J76" s="9"/>
     </row>
-    <row r="77" spans="2:10" ht="18.75" customHeight="1">
+    <row r="77" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2931,7 +2741,7 @@
       </c>
       <c r="J77" s="9"/>
     </row>
-    <row r="78" spans="2:10" ht="18.75" customHeight="1">
+    <row r="78" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2944,7 +2754,7 @@
       </c>
       <c r="J78" s="9"/>
     </row>
-    <row r="79" spans="2:10" ht="18.75" customHeight="1">
+    <row r="79" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2957,7 +2767,7 @@
       </c>
       <c r="J79" s="9"/>
     </row>
-    <row r="80" spans="2:10" ht="18.75" customHeight="1">
+    <row r="80" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2970,7 +2780,7 @@
       </c>
       <c r="J80" s="9"/>
     </row>
-    <row r="81" spans="2:10" ht="18.75" customHeight="1">
+    <row r="81" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2983,7 +2793,7 @@
       </c>
       <c r="J81" s="9"/>
     </row>
-    <row r="82" spans="2:10" ht="18.75" customHeight="1">
+    <row r="82" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2996,7 +2806,7 @@
       </c>
       <c r="J82" s="9"/>
     </row>
-    <row r="83" spans="2:10" ht="18.75" customHeight="1">
+    <row r="83" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3009,7 +2819,7 @@
       </c>
       <c r="J83" s="9"/>
     </row>
-    <row r="84" spans="2:10" ht="18.75" customHeight="1">
+    <row r="84" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3022,7 +2832,7 @@
       </c>
       <c r="J84" s="9"/>
     </row>
-    <row r="85" spans="2:10" ht="18.75" customHeight="1">
+    <row r="85" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3035,7 +2845,7 @@
       </c>
       <c r="J85" s="9"/>
     </row>
-    <row r="86" spans="2:10" ht="18.75" customHeight="1">
+    <row r="86" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3048,7 +2858,7 @@
       </c>
       <c r="J86" s="9"/>
     </row>
-    <row r="87" spans="2:10" ht="18.75" customHeight="1">
+    <row r="87" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3061,7 +2871,7 @@
       </c>
       <c r="J87" s="9"/>
     </row>
-    <row r="88" spans="2:10" ht="18.75" customHeight="1">
+    <row r="88" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3074,7 +2884,7 @@
       </c>
       <c r="J88" s="9"/>
     </row>
-    <row r="89" spans="2:10" ht="18.75" customHeight="1">
+    <row r="89" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3087,7 +2897,7 @@
       </c>
       <c r="J89" s="9"/>
     </row>
-    <row r="90" spans="2:10" ht="18.75" customHeight="1">
+    <row r="90" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3100,7 +2910,7 @@
       </c>
       <c r="J90" s="9"/>
     </row>
-    <row r="91" spans="2:10" ht="18.75" customHeight="1">
+    <row r="91" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3113,7 +2923,7 @@
       </c>
       <c r="J91" s="9"/>
     </row>
-    <row r="92" spans="2:10" ht="18.75" customHeight="1">
+    <row r="92" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3126,7 +2936,7 @@
       </c>
       <c r="J92" s="9"/>
     </row>
-    <row r="93" spans="2:10" ht="18.75" customHeight="1">
+    <row r="93" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3139,7 +2949,7 @@
       </c>
       <c r="J93" s="9"/>
     </row>
-    <row r="94" spans="2:10" ht="18.75" customHeight="1">
+    <row r="94" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3152,7 +2962,7 @@
       </c>
       <c r="J94" s="9"/>
     </row>
-    <row r="95" spans="2:10" ht="18.75" customHeight="1">
+    <row r="95" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3165,7 +2975,7 @@
       </c>
       <c r="J95" s="9"/>
     </row>
-    <row r="96" spans="2:10" ht="18.75" customHeight="1">
+    <row r="96" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3178,7 +2988,7 @@
       </c>
       <c r="J96" s="9"/>
     </row>
-    <row r="97" spans="2:10" ht="18.75" customHeight="1">
+    <row r="97" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3191,7 +3001,7 @@
       </c>
       <c r="J97" s="9"/>
     </row>
-    <row r="98" spans="2:10" ht="18.75" customHeight="1">
+    <row r="98" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3204,7 +3014,7 @@
       </c>
       <c r="J98" s="9"/>
     </row>
-    <row r="99" spans="2:10" ht="18.75" customHeight="1">
+    <row r="99" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3217,7 +3027,7 @@
       </c>
       <c r="J99" s="9"/>
     </row>
-    <row r="100" spans="2:10" ht="18.75" customHeight="1">
+    <row r="100" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3230,7 +3040,7 @@
       </c>
       <c r="J100" s="9"/>
     </row>
-    <row r="101" spans="2:10" ht="18.75" customHeight="1">
+    <row r="101" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3243,7 +3053,7 @@
       </c>
       <c r="J101" s="9"/>
     </row>
-    <row r="102" spans="2:10" ht="18.75" customHeight="1">
+    <row r="102" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3256,7 +3066,7 @@
       </c>
       <c r="J102" s="9"/>
     </row>
-    <row r="103" spans="2:10" ht="18.75" customHeight="1">
+    <row r="103" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3269,7 +3079,7 @@
       </c>
       <c r="J103" s="9"/>
     </row>
-    <row r="104" spans="2:10" ht="18.75" customHeight="1">
+    <row r="104" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3282,7 +3092,7 @@
       </c>
       <c r="J104" s="9"/>
     </row>
-    <row r="105" spans="2:10" ht="18.75" customHeight="1">
+    <row r="105" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3295,7 +3105,7 @@
       </c>
       <c r="J105" s="9"/>
     </row>
-    <row r="106" spans="2:10" ht="18.75" customHeight="1">
+    <row r="106" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3308,7 +3118,7 @@
       </c>
       <c r="J106" s="9"/>
     </row>
-    <row r="107" spans="2:10" ht="18.75" customHeight="1">
+    <row r="107" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3321,7 +3131,7 @@
       </c>
       <c r="J107" s="9"/>
     </row>
-    <row r="108" spans="2:10" ht="18.75" customHeight="1">
+    <row r="108" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3334,7 +3144,7 @@
       </c>
       <c r="J108" s="9"/>
     </row>
-    <row r="109" spans="2:10" ht="18.75" customHeight="1">
+    <row r="109" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3347,7 +3157,7 @@
       </c>
       <c r="J109" s="9"/>
     </row>
-    <row r="110" spans="2:10" ht="18.75" customHeight="1">
+    <row r="110" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3360,7 +3170,7 @@
       </c>
       <c r="J110" s="9"/>
     </row>
-    <row r="111" spans="2:10" ht="18.75" customHeight="1">
+    <row r="111" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3373,7 +3183,7 @@
       </c>
       <c r="J111" s="9"/>
     </row>
-    <row r="112" spans="2:10" ht="18.75" customHeight="1">
+    <row r="112" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3386,7 +3196,7 @@
       </c>
       <c r="J112" s="9"/>
     </row>
-    <row r="113" spans="2:10" ht="18.75" customHeight="1">
+    <row r="113" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3399,7 +3209,7 @@
       </c>
       <c r="J113" s="9"/>
     </row>
-    <row r="114" spans="2:10" ht="18.75" customHeight="1">
+    <row r="114" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3412,7 +3222,7 @@
       </c>
       <c r="J114" s="9"/>
     </row>
-    <row r="115" spans="2:10" ht="18.75" customHeight="1">
+    <row r="115" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3425,7 +3235,7 @@
       </c>
       <c r="J115" s="9"/>
     </row>
-    <row r="116" spans="2:10" ht="18.75" customHeight="1">
+    <row r="116" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3438,7 +3248,7 @@
       </c>
       <c r="J116" s="9"/>
     </row>
-    <row r="117" spans="2:10" ht="18.75" customHeight="1">
+    <row r="117" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3451,7 +3261,7 @@
       </c>
       <c r="J117" s="9"/>
     </row>
-    <row r="118" spans="2:10" ht="18.75" customHeight="1">
+    <row r="118" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3464,7 +3274,7 @@
       </c>
       <c r="J118" s="9"/>
     </row>
-    <row r="119" spans="2:10" ht="18.75" customHeight="1">
+    <row r="119" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3477,7 +3287,7 @@
       </c>
       <c r="J119" s="9"/>
     </row>
-    <row r="120" spans="2:10" ht="18.75" customHeight="1">
+    <row r="120" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3490,7 +3300,7 @@
       </c>
       <c r="J120" s="9"/>
     </row>
-    <row r="121" spans="2:10" ht="18.75" customHeight="1">
+    <row r="121" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3503,7 +3313,7 @@
       </c>
       <c r="J121" s="9"/>
     </row>
-    <row r="122" spans="2:10" ht="18.75" customHeight="1">
+    <row r="122" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3516,7 +3326,7 @@
       </c>
       <c r="J122" s="9"/>
     </row>
-    <row r="123" spans="2:10" ht="18.75" customHeight="1">
+    <row r="123" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3529,7 +3339,7 @@
       </c>
       <c r="J123" s="9"/>
     </row>
-    <row r="124" spans="2:10" ht="18.75" customHeight="1">
+    <row r="124" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3542,7 +3352,7 @@
       </c>
       <c r="J124" s="9"/>
     </row>
-    <row r="125" spans="2:10" ht="18.75" customHeight="1">
+    <row r="125" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3555,7 +3365,7 @@
       </c>
       <c r="J125" s="9"/>
     </row>
-    <row r="126" spans="2:10" ht="18.75" customHeight="1">
+    <row r="126" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3568,7 +3378,7 @@
       </c>
       <c r="J126" s="9"/>
     </row>
-    <row r="127" spans="2:10" ht="18.75" customHeight="1">
+    <row r="127" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3581,7 +3391,7 @@
       </c>
       <c r="J127" s="9"/>
     </row>
-    <row r="128" spans="2:10" ht="18.75" customHeight="1">
+    <row r="128" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3594,7 +3404,7 @@
       </c>
       <c r="J128" s="9"/>
     </row>
-    <row r="129" spans="2:10" ht="18.75" customHeight="1">
+    <row r="129" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3607,7 +3417,7 @@
       </c>
       <c r="J129" s="9"/>
     </row>
-    <row r="130" spans="2:10" ht="18.75" customHeight="1">
+    <row r="130" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3620,7 +3430,7 @@
       </c>
       <c r="J130" s="9"/>
     </row>
-    <row r="131" spans="2:10" ht="18.75" customHeight="1">
+    <row r="131" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3633,7 +3443,7 @@
       </c>
       <c r="J131" s="9"/>
     </row>
-    <row r="132" spans="2:10" ht="18.75" customHeight="1">
+    <row r="132" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3646,7 +3456,7 @@
       </c>
       <c r="J132" s="9"/>
     </row>
-    <row r="133" spans="2:10" ht="18.75" customHeight="1">
+    <row r="133" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3659,7 +3469,7 @@
       </c>
       <c r="J133" s="9"/>
     </row>
-    <row r="134" spans="2:10" ht="18.75" customHeight="1">
+    <row r="134" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3672,7 +3482,7 @@
       </c>
       <c r="J134" s="9"/>
     </row>
-    <row r="135" spans="2:10" ht="18.75" customHeight="1">
+    <row r="135" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3685,7 +3495,7 @@
       </c>
       <c r="J135" s="9"/>
     </row>
-    <row r="136" spans="2:10" ht="18.75" customHeight="1">
+    <row r="136" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3698,7 +3508,7 @@
       </c>
       <c r="J136" s="9"/>
     </row>
-    <row r="137" spans="2:10" ht="18.75" customHeight="1">
+    <row r="137" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="16" t="str">
         <f t="shared" ref="B137:B199" si="4">IF(C137="","",B136+1)</f>
         <v/>
@@ -3711,7 +3521,7 @@
       </c>
       <c r="J137" s="9"/>
     </row>
-    <row r="138" spans="2:10" ht="18.75" customHeight="1">
+    <row r="138" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3724,7 +3534,7 @@
       </c>
       <c r="J138" s="9"/>
     </row>
-    <row r="139" spans="2:10" ht="18.75" customHeight="1">
+    <row r="139" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3737,7 +3547,7 @@
       </c>
       <c r="J139" s="9"/>
     </row>
-    <row r="140" spans="2:10" ht="18.75" customHeight="1">
+    <row r="140" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3750,7 +3560,7 @@
       </c>
       <c r="J140" s="9"/>
     </row>
-    <row r="141" spans="2:10" ht="18.75" customHeight="1">
+    <row r="141" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3763,7 +3573,7 @@
       </c>
       <c r="J141" s="9"/>
     </row>
-    <row r="142" spans="2:10" ht="18.75" customHeight="1">
+    <row r="142" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3776,7 +3586,7 @@
       </c>
       <c r="J142" s="9"/>
     </row>
-    <row r="143" spans="2:10" ht="18.75" customHeight="1">
+    <row r="143" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3789,7 +3599,7 @@
       </c>
       <c r="J143" s="9"/>
     </row>
-    <row r="144" spans="2:10" ht="18.75" customHeight="1">
+    <row r="144" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3802,7 +3612,7 @@
       </c>
       <c r="J144" s="9"/>
     </row>
-    <row r="145" spans="2:10" ht="18.75" customHeight="1">
+    <row r="145" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3815,7 +3625,7 @@
       </c>
       <c r="J145" s="9"/>
     </row>
-    <row r="146" spans="2:10" ht="18.75" customHeight="1">
+    <row r="146" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3828,7 +3638,7 @@
       </c>
       <c r="J146" s="9"/>
     </row>
-    <row r="147" spans="2:10" ht="18.75" customHeight="1">
+    <row r="147" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3841,7 +3651,7 @@
       </c>
       <c r="J147" s="9"/>
     </row>
-    <row r="148" spans="2:10" ht="18.75" customHeight="1">
+    <row r="148" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3854,7 +3664,7 @@
       </c>
       <c r="J148" s="9"/>
     </row>
-    <row r="149" spans="2:10" ht="18.75" customHeight="1">
+    <row r="149" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3867,7 +3677,7 @@
       </c>
       <c r="J149" s="9"/>
     </row>
-    <row r="150" spans="2:10" ht="18.75" customHeight="1">
+    <row r="150" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3880,7 +3690,7 @@
       </c>
       <c r="J150" s="9"/>
     </row>
-    <row r="151" spans="2:10" ht="18.75" customHeight="1">
+    <row r="151" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3893,7 +3703,7 @@
       </c>
       <c r="J151" s="9"/>
     </row>
-    <row r="152" spans="2:10" ht="18.75" customHeight="1">
+    <row r="152" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3906,7 +3716,7 @@
       </c>
       <c r="J152" s="9"/>
     </row>
-    <row r="153" spans="2:10" ht="18.75" customHeight="1">
+    <row r="153" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3919,7 +3729,7 @@
       </c>
       <c r="J153" s="9"/>
     </row>
-    <row r="154" spans="2:10" ht="18.75" customHeight="1">
+    <row r="154" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3932,7 +3742,7 @@
       </c>
       <c r="J154" s="9"/>
     </row>
-    <row r="155" spans="2:10" ht="18.75" customHeight="1">
+    <row r="155" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3945,7 +3755,7 @@
       </c>
       <c r="J155" s="9"/>
     </row>
-    <row r="156" spans="2:10" ht="18.75" customHeight="1">
+    <row r="156" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3958,7 +3768,7 @@
       </c>
       <c r="J156" s="9"/>
     </row>
-    <row r="157" spans="2:10" ht="18.75" customHeight="1">
+    <row r="157" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3971,7 +3781,7 @@
       </c>
       <c r="J157" s="9"/>
     </row>
-    <row r="158" spans="2:10" ht="18.75" customHeight="1">
+    <row r="158" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3984,7 +3794,7 @@
       </c>
       <c r="J158" s="9"/>
     </row>
-    <row r="159" spans="2:10" ht="18.75" customHeight="1">
+    <row r="159" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3997,7 +3807,7 @@
       </c>
       <c r="J159" s="9"/>
     </row>
-    <row r="160" spans="2:10" ht="18.75" customHeight="1">
+    <row r="160" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4010,7 +3820,7 @@
       </c>
       <c r="J160" s="9"/>
     </row>
-    <row r="161" spans="2:10" ht="18.75" customHeight="1">
+    <row r="161" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4023,7 +3833,7 @@
       </c>
       <c r="J161" s="9"/>
     </row>
-    <row r="162" spans="2:10" ht="18.75" customHeight="1">
+    <row r="162" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4036,7 +3846,7 @@
       </c>
       <c r="J162" s="9"/>
     </row>
-    <row r="163" spans="2:10" ht="18.75" customHeight="1">
+    <row r="163" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4049,7 +3859,7 @@
       </c>
       <c r="J163" s="9"/>
     </row>
-    <row r="164" spans="2:10" ht="18.75" customHeight="1">
+    <row r="164" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4062,7 +3872,7 @@
       </c>
       <c r="J164" s="9"/>
     </row>
-    <row r="165" spans="2:10" ht="18.75" customHeight="1">
+    <row r="165" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4075,7 +3885,7 @@
       </c>
       <c r="J165" s="9"/>
     </row>
-    <row r="166" spans="2:10" ht="18.75" customHeight="1">
+    <row r="166" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4088,7 +3898,7 @@
       </c>
       <c r="J166" s="9"/>
     </row>
-    <row r="167" spans="2:10" ht="18.75" customHeight="1">
+    <row r="167" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4101,7 +3911,7 @@
       </c>
       <c r="J167" s="9"/>
     </row>
-    <row r="168" spans="2:10" ht="18.75" customHeight="1">
+    <row r="168" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4114,7 +3924,7 @@
       </c>
       <c r="J168" s="9"/>
     </row>
-    <row r="169" spans="2:10" ht="18.75" customHeight="1">
+    <row r="169" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4127,7 +3937,7 @@
       </c>
       <c r="J169" s="9"/>
     </row>
-    <row r="170" spans="2:10" ht="18.75" customHeight="1">
+    <row r="170" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4140,7 +3950,7 @@
       </c>
       <c r="J170" s="9"/>
     </row>
-    <row r="171" spans="2:10" ht="18.75" customHeight="1">
+    <row r="171" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4153,7 +3963,7 @@
       </c>
       <c r="J171" s="9"/>
     </row>
-    <row r="172" spans="2:10" ht="18.75" customHeight="1">
+    <row r="172" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4166,7 +3976,7 @@
       </c>
       <c r="J172" s="9"/>
     </row>
-    <row r="173" spans="2:10" ht="18.75" customHeight="1">
+    <row r="173" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4179,7 +3989,7 @@
       </c>
       <c r="J173" s="9"/>
     </row>
-    <row r="174" spans="2:10" ht="18.75" customHeight="1">
+    <row r="174" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4192,7 +4002,7 @@
       </c>
       <c r="J174" s="9"/>
     </row>
-    <row r="175" spans="2:10" ht="18.75" customHeight="1">
+    <row r="175" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4205,7 +4015,7 @@
       </c>
       <c r="J175" s="9"/>
     </row>
-    <row r="176" spans="2:10" ht="18.75" customHeight="1">
+    <row r="176" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4218,7 +4028,7 @@
       </c>
       <c r="J176" s="9"/>
     </row>
-    <row r="177" spans="2:10" ht="18.75" customHeight="1">
+    <row r="177" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4231,7 +4041,7 @@
       </c>
       <c r="J177" s="9"/>
     </row>
-    <row r="178" spans="2:10" ht="18.75" customHeight="1">
+    <row r="178" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4244,7 +4054,7 @@
       </c>
       <c r="J178" s="9"/>
     </row>
-    <row r="179" spans="2:10" ht="18.75" customHeight="1">
+    <row r="179" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4257,7 +4067,7 @@
       </c>
       <c r="J179" s="9"/>
     </row>
-    <row r="180" spans="2:10" ht="18.75" customHeight="1">
+    <row r="180" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4270,7 +4080,7 @@
       </c>
       <c r="J180" s="9"/>
     </row>
-    <row r="181" spans="2:10" ht="18.75" customHeight="1">
+    <row r="181" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4283,7 +4093,7 @@
       </c>
       <c r="J181" s="9"/>
     </row>
-    <row r="182" spans="2:10" ht="18.75" customHeight="1">
+    <row r="182" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4296,7 +4106,7 @@
       </c>
       <c r="J182" s="9"/>
     </row>
-    <row r="183" spans="2:10" ht="18.75" customHeight="1">
+    <row r="183" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4309,7 +4119,7 @@
       </c>
       <c r="J183" s="9"/>
     </row>
-    <row r="184" spans="2:10" ht="18.75" customHeight="1">
+    <row r="184" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4322,7 +4132,7 @@
       </c>
       <c r="J184" s="9"/>
     </row>
-    <row r="185" spans="2:10" ht="18.75" customHeight="1">
+    <row r="185" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4335,7 +4145,7 @@
       </c>
       <c r="J185" s="9"/>
     </row>
-    <row r="186" spans="2:10" ht="18.75" customHeight="1">
+    <row r="186" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4348,7 +4158,7 @@
       </c>
       <c r="J186" s="9"/>
     </row>
-    <row r="187" spans="2:10" ht="18.75" customHeight="1">
+    <row r="187" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4361,7 +4171,7 @@
       </c>
       <c r="J187" s="9"/>
     </row>
-    <row r="188" spans="2:10" ht="18.75" customHeight="1">
+    <row r="188" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4374,7 +4184,7 @@
       </c>
       <c r="J188" s="9"/>
     </row>
-    <row r="189" spans="2:10" ht="18.75" customHeight="1">
+    <row r="189" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4387,7 +4197,7 @@
       </c>
       <c r="J189" s="9"/>
     </row>
-    <row r="190" spans="2:10" ht="18.75" customHeight="1">
+    <row r="190" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4400,7 +4210,7 @@
       </c>
       <c r="J190" s="9"/>
     </row>
-    <row r="191" spans="2:10" ht="18.75" customHeight="1">
+    <row r="191" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4413,7 +4223,7 @@
       </c>
       <c r="J191" s="9"/>
     </row>
-    <row r="192" spans="2:10" ht="18.75" customHeight="1">
+    <row r="192" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4426,7 +4236,7 @@
       </c>
       <c r="J192" s="9"/>
     </row>
-    <row r="193" spans="2:10" ht="18.75" customHeight="1">
+    <row r="193" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4439,7 +4249,7 @@
       </c>
       <c r="J193" s="9"/>
     </row>
-    <row r="194" spans="2:10" ht="18.75" customHeight="1">
+    <row r="194" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4452,7 +4262,7 @@
       </c>
       <c r="J194" s="9"/>
     </row>
-    <row r="195" spans="2:10" ht="18.75" customHeight="1">
+    <row r="195" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4465,7 +4275,7 @@
       </c>
       <c r="J195" s="9"/>
     </row>
-    <row r="196" spans="2:10" ht="18.75" customHeight="1">
+    <row r="196" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4478,7 +4288,7 @@
       </c>
       <c r="J196" s="9"/>
     </row>
-    <row r="197" spans="2:10" ht="18.75" customHeight="1">
+    <row r="197" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4491,7 +4301,7 @@
       </c>
       <c r="J197" s="9"/>
     </row>
-    <row r="198" spans="2:10" ht="18.75" customHeight="1">
+    <row r="198" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4504,7 +4314,7 @@
       </c>
       <c r="J198" s="9"/>
     </row>
-    <row r="199" spans="2:10" ht="18.75" customHeight="1">
+    <row r="199" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4517,7 +4327,7 @@
       </c>
       <c r="J199" s="9"/>
     </row>
-    <row r="200" spans="2:10" ht="18.75" customHeight="1">
+    <row r="200" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="16"/>
       <c r="G200" s="9"/>
       <c r="H200" s="9"/>
@@ -4527,7 +4337,7 @@
       </c>
       <c r="J200" s="9"/>
     </row>
-    <row r="201" spans="2:10" ht="18.75" customHeight="1">
+    <row r="201" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="16"/>
       <c r="G201" s="9"/>
       <c r="H201" s="9"/>
@@ -4537,7 +4347,7 @@
       </c>
       <c r="J201" s="9"/>
     </row>
-    <row r="202" spans="2:10" ht="18.75" customHeight="1">
+    <row r="202" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="16"/>
       <c r="G202" s="9"/>
       <c r="H202" s="9"/>
@@ -4547,7 +4357,7 @@
       </c>
       <c r="J202" s="9"/>
     </row>
-    <row r="203" spans="2:10" ht="18.75" customHeight="1">
+    <row r="203" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="16"/>
       <c r="G203" s="9"/>
       <c r="H203" s="9"/>
@@ -4557,7 +4367,7 @@
       </c>
       <c r="J203" s="9"/>
     </row>
-    <row r="204" spans="2:10" ht="18.75" customHeight="1">
+    <row r="204" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="16"/>
       <c r="G204" s="9"/>
       <c r="H204" s="9"/>
@@ -4567,7 +4377,7 @@
       </c>
       <c r="J204" s="9"/>
     </row>
-    <row r="205" spans="2:10" ht="18.75" customHeight="1">
+    <row r="205" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="16"/>
       <c r="G205" s="9"/>
       <c r="H205" s="9"/>
@@ -4577,7 +4387,7 @@
       </c>
       <c r="J205" s="9"/>
     </row>
-    <row r="206" spans="2:10" ht="18.75" customHeight="1">
+    <row r="206" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="16"/>
       <c r="G206" s="9"/>
       <c r="H206" s="9"/>
@@ -4587,7 +4397,7 @@
       </c>
       <c r="J206" s="9"/>
     </row>
-    <row r="207" spans="2:10" ht="18.75" customHeight="1">
+    <row r="207" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="16"/>
       <c r="G207" s="9"/>
       <c r="H207" s="9"/>
@@ -4597,7 +4407,7 @@
       </c>
       <c r="J207" s="9"/>
     </row>
-    <row r="208" spans="2:10" ht="18.75" customHeight="1">
+    <row r="208" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="16"/>
       <c r="G208" s="9"/>
       <c r="H208" s="9"/>
@@ -4607,7 +4417,7 @@
       </c>
       <c r="J208" s="9"/>
     </row>
-    <row r="209" spans="2:10" ht="18.75" customHeight="1">
+    <row r="209" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="16"/>
       <c r="G209" s="9"/>
       <c r="H209" s="9"/>
@@ -4617,7 +4427,7 @@
       </c>
       <c r="J209" s="9"/>
     </row>
-    <row r="210" spans="2:10" ht="18.75" customHeight="1">
+    <row r="210" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="16"/>
       <c r="G210" s="9"/>
       <c r="H210" s="9"/>
@@ -4627,7 +4437,7 @@
       </c>
       <c r="J210" s="9"/>
     </row>
-    <row r="211" spans="2:10" ht="18.75" customHeight="1">
+    <row r="211" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="16"/>
       <c r="G211" s="9"/>
       <c r="H211" s="9"/>
@@ -4637,7 +4447,7 @@
       </c>
       <c r="J211" s="9"/>
     </row>
-    <row r="212" spans="2:10" ht="18.75" customHeight="1">
+    <row r="212" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="16"/>
       <c r="G212" s="9"/>
       <c r="H212" s="9"/>
@@ -4647,7 +4457,7 @@
       </c>
       <c r="J212" s="9"/>
     </row>
-    <row r="213" spans="2:10" ht="18.75" customHeight="1">
+    <row r="213" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="16"/>
       <c r="G213" s="9"/>
       <c r="H213" s="9"/>
@@ -4657,7 +4467,7 @@
       </c>
       <c r="J213" s="9"/>
     </row>
-    <row r="214" spans="2:10" ht="18.75" customHeight="1">
+    <row r="214" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="16"/>
       <c r="G214" s="9"/>
       <c r="H214" s="9"/>
@@ -4667,7 +4477,7 @@
       </c>
       <c r="J214" s="9"/>
     </row>
-    <row r="215" spans="2:10" ht="18.75" customHeight="1">
+    <row r="215" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="16"/>
       <c r="G215" s="9"/>
       <c r="H215" s="9"/>
@@ -4677,7 +4487,7 @@
       </c>
       <c r="J215" s="9"/>
     </row>
-    <row r="216" spans="2:10" ht="18.75" customHeight="1">
+    <row r="216" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="16"/>
       <c r="G216" s="9"/>
       <c r="H216" s="9"/>
@@ -4687,7 +4497,7 @@
       </c>
       <c r="J216" s="9"/>
     </row>
-    <row r="217" spans="2:10" ht="18.75" customHeight="1">
+    <row r="217" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="16"/>
       <c r="G217" s="9"/>
       <c r="H217" s="9"/>
@@ -4697,7 +4507,7 @@
       </c>
       <c r="J217" s="9"/>
     </row>
-    <row r="218" spans="2:10" ht="18.75" customHeight="1">
+    <row r="218" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="16"/>
       <c r="G218" s="9"/>
       <c r="H218" s="9"/>
@@ -4707,7 +4517,7 @@
       </c>
       <c r="J218" s="9"/>
     </row>
-    <row r="219" spans="2:10" ht="18.75" customHeight="1">
+    <row r="219" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="16"/>
       <c r="G219" s="9"/>
       <c r="H219" s="9"/>
@@ -4717,7 +4527,7 @@
       </c>
       <c r="J219" s="9"/>
     </row>
-    <row r="220" spans="2:10" ht="18.75" customHeight="1">
+    <row r="220" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B220" s="16"/>
       <c r="G220" s="9"/>
       <c r="H220" s="9"/>
@@ -4727,7 +4537,7 @@
       </c>
       <c r="J220" s="9"/>
     </row>
-    <row r="221" spans="2:10" ht="18.75" customHeight="1">
+    <row r="221" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B221" s="16"/>
       <c r="G221" s="9"/>
       <c r="H221" s="9"/>
@@ -4737,7 +4547,7 @@
       </c>
       <c r="J221" s="9"/>
     </row>
-    <row r="222" spans="2:10" ht="18.75" customHeight="1">
+    <row r="222" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="16"/>
       <c r="G222" s="9"/>
       <c r="H222" s="9"/>
@@ -4747,7 +4557,7 @@
       </c>
       <c r="J222" s="9"/>
     </row>
-    <row r="223" spans="2:10" ht="18.75" customHeight="1">
+    <row r="223" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223" s="16"/>
       <c r="G223" s="9"/>
       <c r="H223" s="9"/>
@@ -4757,7 +4567,7 @@
       </c>
       <c r="J223" s="9"/>
     </row>
-    <row r="224" spans="2:10" ht="18.75" customHeight="1">
+    <row r="224" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="16"/>
       <c r="G224" s="9"/>
       <c r="H224" s="9"/>
@@ -4767,7 +4577,7 @@
       </c>
       <c r="J224" s="9"/>
     </row>
-    <row r="225" spans="2:10" ht="18.75" customHeight="1">
+    <row r="225" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B225" s="16"/>
       <c r="G225" s="9"/>
       <c r="H225" s="9"/>
@@ -4777,838 +4587,838 @@
       </c>
       <c r="J225" s="9"/>
     </row>
-    <row r="226" spans="2:10" ht="18.75" customHeight="1">
+    <row r="226" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="16"/>
       <c r="G226" s="9"/>
       <c r="H226" s="9"/>
       <c r="J226" s="9"/>
     </row>
-    <row r="227" spans="2:10" ht="18.75" customHeight="1">
+    <row r="227" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G227" s="9"/>
       <c r="H227" s="9"/>
       <c r="J227" s="9"/>
     </row>
-    <row r="228" spans="2:10" ht="18.75" customHeight="1">
+    <row r="228" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G228" s="9"/>
       <c r="H228" s="9"/>
       <c r="J228" s="9"/>
     </row>
-    <row r="229" spans="2:10" ht="18.75" customHeight="1">
+    <row r="229" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G229" s="9"/>
       <c r="H229" s="9"/>
       <c r="J229" s="9"/>
     </row>
-    <row r="230" spans="2:10" ht="18.75" customHeight="1">
+    <row r="230" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G230" s="9"/>
       <c r="H230" s="9"/>
       <c r="J230" s="9"/>
     </row>
-    <row r="231" spans="2:10" ht="18.75" customHeight="1">
+    <row r="231" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G231" s="9"/>
       <c r="H231" s="9"/>
       <c r="J231" s="9"/>
     </row>
-    <row r="232" spans="2:10" ht="18.75" customHeight="1">
+    <row r="232" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G232" s="9"/>
       <c r="H232" s="9"/>
       <c r="J232" s="9"/>
     </row>
-    <row r="233" spans="2:10" ht="18.75" customHeight="1">
+    <row r="233" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G233" s="9"/>
       <c r="H233" s="9"/>
       <c r="J233" s="9"/>
     </row>
-    <row r="234" spans="2:10" ht="18.75" customHeight="1">
+    <row r="234" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G234" s="9"/>
       <c r="H234" s="9"/>
       <c r="J234" s="9"/>
     </row>
-    <row r="235" spans="2:10" ht="18.75" customHeight="1">
+    <row r="235" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G235" s="9"/>
       <c r="H235" s="9"/>
       <c r="J235" s="9"/>
     </row>
-    <row r="236" spans="2:10" ht="18.75" customHeight="1">
+    <row r="236" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G236" s="9"/>
       <c r="H236" s="9"/>
       <c r="J236" s="9"/>
     </row>
-    <row r="237" spans="2:10" ht="18.75" customHeight="1">
+    <row r="237" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G237" s="9"/>
       <c r="H237" s="9"/>
       <c r="J237" s="9"/>
     </row>
-    <row r="238" spans="2:10" ht="18.75" customHeight="1">
+    <row r="238" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G238" s="9"/>
       <c r="H238" s="9"/>
       <c r="J238" s="9"/>
     </row>
-    <row r="239" spans="2:10" ht="18.75" customHeight="1">
+    <row r="239" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G239" s="9"/>
       <c r="H239" s="9"/>
       <c r="J239" s="9"/>
     </row>
-    <row r="240" spans="2:10" ht="18.75" customHeight="1">
+    <row r="240" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G240" s="9"/>
       <c r="H240" s="9"/>
       <c r="J240" s="9"/>
     </row>
-    <row r="241" spans="7:10" ht="18.75" customHeight="1">
+    <row r="241" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G241" s="9"/>
       <c r="H241" s="9"/>
       <c r="J241" s="9"/>
     </row>
-    <row r="242" spans="7:10" ht="18.75" customHeight="1">
+    <row r="242" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G242" s="9"/>
       <c r="H242" s="9"/>
       <c r="J242" s="9"/>
     </row>
-    <row r="243" spans="7:10" ht="18.75" customHeight="1">
+    <row r="243" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G243" s="9"/>
       <c r="H243" s="9"/>
       <c r="J243" s="9"/>
     </row>
-    <row r="244" spans="7:10" ht="18.75" customHeight="1">
+    <row r="244" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G244" s="9"/>
       <c r="H244" s="9"/>
       <c r="J244" s="9"/>
     </row>
-    <row r="245" spans="7:10" ht="18.75" customHeight="1">
+    <row r="245" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G245" s="9"/>
       <c r="H245" s="9"/>
       <c r="J245" s="9"/>
     </row>
-    <row r="246" spans="7:10" ht="18.75" customHeight="1">
+    <row r="246" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G246" s="9"/>
       <c r="H246" s="9"/>
       <c r="J246" s="9"/>
     </row>
-    <row r="247" spans="7:10" ht="18.75" customHeight="1">
+    <row r="247" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G247" s="9"/>
       <c r="H247" s="9"/>
       <c r="J247" s="9"/>
     </row>
-    <row r="248" spans="7:10" ht="18.75" customHeight="1">
+    <row r="248" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G248" s="9"/>
       <c r="H248" s="9"/>
       <c r="J248" s="9"/>
     </row>
-    <row r="249" spans="7:10" ht="18.75" customHeight="1">
+    <row r="249" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G249" s="9"/>
       <c r="H249" s="9"/>
       <c r="J249" s="9"/>
     </row>
-    <row r="250" spans="7:10" ht="18.75" customHeight="1">
+    <row r="250" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G250" s="9"/>
       <c r="H250" s="9"/>
       <c r="J250" s="9"/>
     </row>
-    <row r="251" spans="7:10" ht="18.75" customHeight="1">
+    <row r="251" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G251" s="9"/>
       <c r="H251" s="9"/>
       <c r="J251" s="9"/>
     </row>
-    <row r="252" spans="7:10" ht="18.75" customHeight="1">
+    <row r="252" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G252" s="9"/>
       <c r="H252" s="9"/>
       <c r="J252" s="9"/>
     </row>
-    <row r="253" spans="7:10" ht="18.75" customHeight="1">
+    <row r="253" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G253" s="9"/>
       <c r="H253" s="9"/>
       <c r="J253" s="9"/>
     </row>
-    <row r="254" spans="7:10" ht="18.75" customHeight="1">
+    <row r="254" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G254" s="9"/>
       <c r="H254" s="9"/>
       <c r="J254" s="9"/>
     </row>
-    <row r="255" spans="7:10" ht="18.75" customHeight="1">
+    <row r="255" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G255" s="9"/>
       <c r="H255" s="9"/>
       <c r="J255" s="9"/>
     </row>
-    <row r="256" spans="7:10" ht="18.75" customHeight="1">
+    <row r="256" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G256" s="9"/>
       <c r="H256" s="9"/>
       <c r="J256" s="9"/>
     </row>
-    <row r="257" spans="7:10" ht="18.75" customHeight="1">
+    <row r="257" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G257" s="9"/>
       <c r="H257" s="9"/>
       <c r="J257" s="9"/>
     </row>
-    <row r="258" spans="7:10" ht="18.75" customHeight="1">
+    <row r="258" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G258" s="9"/>
       <c r="H258" s="9"/>
       <c r="J258" s="9"/>
     </row>
-    <row r="259" spans="7:10" ht="18.75" customHeight="1">
+    <row r="259" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G259" s="9"/>
       <c r="H259" s="9"/>
       <c r="J259" s="9"/>
     </row>
-    <row r="260" spans="7:10" ht="18.75" customHeight="1">
+    <row r="260" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G260" s="9"/>
       <c r="H260" s="9"/>
       <c r="J260" s="9"/>
     </row>
-    <row r="261" spans="7:10" ht="18.75" customHeight="1">
+    <row r="261" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G261" s="9"/>
       <c r="H261" s="9"/>
       <c r="J261" s="9"/>
     </row>
-    <row r="262" spans="7:10" ht="18.75" customHeight="1">
+    <row r="262" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G262" s="9"/>
       <c r="H262" s="9"/>
       <c r="J262" s="9"/>
     </row>
-    <row r="263" spans="7:10" ht="18.75" customHeight="1">
+    <row r="263" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G263" s="9"/>
       <c r="H263" s="9"/>
       <c r="J263" s="9"/>
     </row>
-    <row r="264" spans="7:10" ht="18.75" customHeight="1">
+    <row r="264" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G264" s="9"/>
       <c r="H264" s="9"/>
       <c r="J264" s="9"/>
     </row>
-    <row r="265" spans="7:10" ht="18.75" customHeight="1">
+    <row r="265" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G265" s="9"/>
       <c r="H265" s="9"/>
       <c r="J265" s="9"/>
     </row>
-    <row r="266" spans="7:10" ht="18.75" customHeight="1">
+    <row r="266" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G266" s="9"/>
       <c r="H266" s="9"/>
       <c r="J266" s="9"/>
     </row>
-    <row r="267" spans="7:10" ht="18.75" customHeight="1">
+    <row r="267" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G267" s="9"/>
       <c r="H267" s="9"/>
       <c r="J267" s="9"/>
     </row>
-    <row r="268" spans="7:10" ht="18.75" customHeight="1">
+    <row r="268" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G268" s="9"/>
       <c r="H268" s="9"/>
       <c r="J268" s="9"/>
     </row>
-    <row r="269" spans="7:10" ht="18.75" customHeight="1">
+    <row r="269" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G269" s="9"/>
       <c r="H269" s="9"/>
       <c r="J269" s="9"/>
     </row>
-    <row r="270" spans="7:10" ht="18.75" customHeight="1">
+    <row r="270" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G270" s="9"/>
       <c r="H270" s="9"/>
       <c r="J270" s="9"/>
     </row>
-    <row r="271" spans="7:10" ht="18.75" customHeight="1">
+    <row r="271" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G271" s="9"/>
       <c r="H271" s="9"/>
       <c r="J271" s="9"/>
     </row>
-    <row r="272" spans="7:10" ht="18.75" customHeight="1">
+    <row r="272" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G272" s="9"/>
       <c r="H272" s="9"/>
       <c r="J272" s="9"/>
     </row>
-    <row r="273" spans="7:10" ht="18.75" customHeight="1">
+    <row r="273" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G273" s="9"/>
       <c r="H273" s="9"/>
       <c r="J273" s="9"/>
     </row>
-    <row r="274" spans="7:10" ht="18.75" customHeight="1">
+    <row r="274" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G274" s="9"/>
       <c r="H274" s="9"/>
       <c r="J274" s="9"/>
     </row>
-    <row r="275" spans="7:10" ht="18.75" customHeight="1">
+    <row r="275" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G275" s="9"/>
       <c r="H275" s="9"/>
       <c r="J275" s="9"/>
     </row>
-    <row r="276" spans="7:10" ht="18.75" customHeight="1">
+    <row r="276" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G276" s="9"/>
       <c r="H276" s="9"/>
       <c r="J276" s="9"/>
     </row>
-    <row r="277" spans="7:10" ht="18.75" customHeight="1">
+    <row r="277" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G277" s="9"/>
       <c r="H277" s="9"/>
       <c r="J277" s="9"/>
     </row>
-    <row r="278" spans="7:10" ht="18.75" customHeight="1">
+    <row r="278" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G278" s="9"/>
       <c r="H278" s="9"/>
       <c r="J278" s="9"/>
     </row>
-    <row r="279" spans="7:10" ht="18.75" customHeight="1">
+    <row r="279" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G279" s="9"/>
       <c r="H279" s="9"/>
       <c r="J279" s="9"/>
     </row>
-    <row r="280" spans="7:10" ht="18.75" customHeight="1">
+    <row r="280" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G280" s="9"/>
       <c r="H280" s="9"/>
       <c r="J280" s="9"/>
     </row>
-    <row r="281" spans="7:10" ht="18.75" customHeight="1">
+    <row r="281" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G281" s="9"/>
       <c r="H281" s="9"/>
       <c r="J281" s="9"/>
     </row>
-    <row r="282" spans="7:10" ht="18.75" customHeight="1">
+    <row r="282" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G282" s="9"/>
       <c r="H282" s="9"/>
       <c r="J282" s="9"/>
     </row>
-    <row r="283" spans="7:10" ht="18.75" customHeight="1">
+    <row r="283" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G283" s="9"/>
       <c r="H283" s="9"/>
       <c r="J283" s="9"/>
     </row>
-    <row r="284" spans="7:10" ht="18.75" customHeight="1">
+    <row r="284" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G284" s="9"/>
       <c r="H284" s="9"/>
       <c r="J284" s="9"/>
     </row>
-    <row r="285" spans="7:10" ht="18.75" customHeight="1">
+    <row r="285" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G285" s="9"/>
       <c r="H285" s="9"/>
       <c r="J285" s="9"/>
     </row>
-    <row r="286" spans="7:10" ht="18.75" customHeight="1">
+    <row r="286" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G286" s="9"/>
       <c r="H286" s="9"/>
       <c r="J286" s="9"/>
     </row>
-    <row r="287" spans="7:10" ht="18.75" customHeight="1">
+    <row r="287" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G287" s="9"/>
       <c r="H287" s="9"/>
       <c r="J287" s="9"/>
     </row>
-    <row r="288" spans="7:10" ht="18.75" customHeight="1">
+    <row r="288" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G288" s="9"/>
       <c r="H288" s="9"/>
       <c r="J288" s="9"/>
     </row>
-    <row r="289" spans="7:10" ht="18.75" customHeight="1">
+    <row r="289" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G289" s="9"/>
       <c r="H289" s="9"/>
       <c r="J289" s="9"/>
     </row>
-    <row r="290" spans="7:10" ht="18.75" customHeight="1">
+    <row r="290" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G290" s="9"/>
       <c r="H290" s="9"/>
       <c r="J290" s="9"/>
     </row>
-    <row r="291" spans="7:10" ht="18.75" customHeight="1">
+    <row r="291" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G291" s="9"/>
       <c r="H291" s="9"/>
       <c r="J291" s="9"/>
     </row>
-    <row r="292" spans="7:10" ht="18.75" customHeight="1">
+    <row r="292" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G292" s="9"/>
       <c r="H292" s="9"/>
       <c r="J292" s="9"/>
     </row>
-    <row r="293" spans="7:10" ht="18.75" customHeight="1">
+    <row r="293" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G293" s="9"/>
       <c r="H293" s="9"/>
       <c r="J293" s="9"/>
     </row>
-    <row r="294" spans="7:10" ht="18.75" customHeight="1">
+    <row r="294" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G294" s="9"/>
       <c r="H294" s="9"/>
       <c r="J294" s="9"/>
     </row>
-    <row r="295" spans="7:10" ht="18.75" customHeight="1">
+    <row r="295" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G295" s="9"/>
       <c r="H295" s="9"/>
       <c r="J295" s="9"/>
     </row>
-    <row r="296" spans="7:10" ht="18.75" customHeight="1">
+    <row r="296" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G296" s="9"/>
       <c r="H296" s="9"/>
       <c r="J296" s="9"/>
     </row>
-    <row r="297" spans="7:10" ht="18.75" customHeight="1">
+    <row r="297" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G297" s="9"/>
       <c r="H297" s="9"/>
       <c r="J297" s="9"/>
     </row>
-    <row r="298" spans="7:10" ht="18.75" customHeight="1">
+    <row r="298" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G298" s="9"/>
       <c r="H298" s="9"/>
       <c r="J298" s="9"/>
     </row>
-    <row r="299" spans="7:10" ht="18.75" customHeight="1">
+    <row r="299" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G299" s="9"/>
       <c r="H299" s="9"/>
       <c r="J299" s="9"/>
     </row>
-    <row r="300" spans="7:10" ht="18.75" customHeight="1">
+    <row r="300" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G300" s="9"/>
       <c r="H300" s="9"/>
       <c r="J300" s="9"/>
     </row>
-    <row r="301" spans="7:10" ht="18.75" customHeight="1">
+    <row r="301" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G301" s="9"/>
       <c r="H301" s="9"/>
       <c r="J301" s="9"/>
     </row>
-    <row r="302" spans="7:10" ht="18.75" customHeight="1">
+    <row r="302" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G302" s="9"/>
       <c r="H302" s="9"/>
       <c r="J302" s="9"/>
     </row>
-    <row r="303" spans="7:10" ht="18.75" customHeight="1">
+    <row r="303" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G303" s="9"/>
       <c r="H303" s="9"/>
       <c r="J303" s="9"/>
     </row>
-    <row r="304" spans="7:10" ht="18.75" customHeight="1">
+    <row r="304" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G304" s="9"/>
       <c r="H304" s="9"/>
       <c r="J304" s="9"/>
     </row>
-    <row r="305" spans="7:10" ht="18.75" customHeight="1">
+    <row r="305" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G305" s="9"/>
       <c r="H305" s="9"/>
       <c r="J305" s="9"/>
     </row>
-    <row r="306" spans="7:10" ht="18.75" customHeight="1">
+    <row r="306" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G306" s="9"/>
       <c r="H306" s="9"/>
       <c r="J306" s="9"/>
     </row>
-    <row r="307" spans="7:10" ht="18.75" customHeight="1">
+    <row r="307" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G307" s="9"/>
       <c r="H307" s="9"/>
       <c r="J307" s="9"/>
     </row>
-    <row r="308" spans="7:10" ht="18.75" customHeight="1">
+    <row r="308" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G308" s="9"/>
       <c r="H308" s="9"/>
       <c r="J308" s="9"/>
     </row>
-    <row r="309" spans="7:10" ht="18.75" customHeight="1">
+    <row r="309" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G309" s="9"/>
       <c r="H309" s="9"/>
       <c r="J309" s="9"/>
     </row>
-    <row r="310" spans="7:10" ht="18.75" customHeight="1">
+    <row r="310" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G310" s="9"/>
       <c r="H310" s="9"/>
       <c r="J310" s="9"/>
     </row>
-    <row r="311" spans="7:10" ht="18.75" customHeight="1">
+    <row r="311" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G311" s="9"/>
       <c r="H311" s="9"/>
       <c r="J311" s="9"/>
     </row>
-    <row r="312" spans="7:10" ht="18.75" customHeight="1">
+    <row r="312" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G312" s="9"/>
       <c r="H312" s="9"/>
       <c r="J312" s="9"/>
     </row>
-    <row r="313" spans="7:10" ht="18.75" customHeight="1">
+    <row r="313" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G313" s="9"/>
       <c r="H313" s="9"/>
       <c r="J313" s="9"/>
     </row>
-    <row r="314" spans="7:10" ht="18.75" customHeight="1">
+    <row r="314" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G314" s="9"/>
       <c r="H314" s="9"/>
       <c r="J314" s="9"/>
     </row>
-    <row r="315" spans="7:10" ht="18.75" customHeight="1">
+    <row r="315" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G315" s="9"/>
       <c r="H315" s="9"/>
       <c r="J315" s="9"/>
     </row>
-    <row r="316" spans="7:10" ht="18.75" customHeight="1">
+    <row r="316" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G316" s="9"/>
       <c r="H316" s="9"/>
       <c r="J316" s="9"/>
     </row>
-    <row r="317" spans="7:10" ht="18.75" customHeight="1">
+    <row r="317" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G317" s="9"/>
       <c r="H317" s="9"/>
       <c r="J317" s="9"/>
     </row>
-    <row r="318" spans="7:10" ht="18.75" customHeight="1">
+    <row r="318" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G318" s="9"/>
       <c r="H318" s="9"/>
       <c r="J318" s="9"/>
     </row>
-    <row r="319" spans="7:10" ht="18.75" customHeight="1">
+    <row r="319" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G319" s="9"/>
       <c r="H319" s="9"/>
       <c r="J319" s="9"/>
     </row>
-    <row r="320" spans="7:10" ht="18.75" customHeight="1">
+    <row r="320" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G320" s="9"/>
       <c r="H320" s="9"/>
       <c r="J320" s="9"/>
     </row>
-    <row r="321" spans="7:10" ht="18.75" customHeight="1">
+    <row r="321" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G321" s="9"/>
       <c r="H321" s="9"/>
       <c r="J321" s="9"/>
     </row>
-    <row r="322" spans="7:10" ht="18.75" customHeight="1">
+    <row r="322" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G322" s="9"/>
       <c r="H322" s="9"/>
       <c r="J322" s="9"/>
     </row>
-    <row r="323" spans="7:10" ht="18.75" customHeight="1">
+    <row r="323" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G323" s="9"/>
       <c r="H323" s="9"/>
       <c r="J323" s="9"/>
     </row>
-    <row r="324" spans="7:10" ht="18.75" customHeight="1">
+    <row r="324" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G324" s="9"/>
       <c r="H324" s="9"/>
       <c r="J324" s="9"/>
     </row>
-    <row r="325" spans="7:10" ht="18.75" customHeight="1">
+    <row r="325" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G325" s="9"/>
       <c r="H325" s="9"/>
       <c r="J325" s="9"/>
     </row>
-    <row r="326" spans="7:10" ht="18.75" customHeight="1">
+    <row r="326" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G326" s="9"/>
       <c r="H326" s="9"/>
       <c r="J326" s="9"/>
     </row>
-    <row r="327" spans="7:10" ht="18.75" customHeight="1">
+    <row r="327" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G327" s="9"/>
       <c r="H327" s="9"/>
       <c r="J327" s="9"/>
     </row>
-    <row r="328" spans="7:10" ht="18.75" customHeight="1">
+    <row r="328" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G328" s="9"/>
       <c r="H328" s="9"/>
       <c r="J328" s="9"/>
     </row>
-    <row r="329" spans="7:10" ht="18.75" customHeight="1">
+    <row r="329" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G329" s="9"/>
       <c r="H329" s="9"/>
       <c r="J329" s="9"/>
     </row>
-    <row r="330" spans="7:10" ht="18.75" customHeight="1">
+    <row r="330" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G330" s="9"/>
       <c r="H330" s="9"/>
       <c r="J330" s="9"/>
     </row>
-    <row r="331" spans="7:10" ht="18.75" customHeight="1">
+    <row r="331" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G331" s="9"/>
       <c r="H331" s="9"/>
       <c r="J331" s="9"/>
     </row>
-    <row r="332" spans="7:10" ht="18.75" customHeight="1">
+    <row r="332" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G332" s="9"/>
       <c r="H332" s="9"/>
       <c r="J332" s="9"/>
     </row>
-    <row r="333" spans="7:10" ht="18.75" customHeight="1">
+    <row r="333" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G333" s="9"/>
       <c r="H333" s="9"/>
       <c r="J333" s="9"/>
     </row>
-    <row r="334" spans="7:10" ht="18.75" customHeight="1">
+    <row r="334" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G334" s="9"/>
       <c r="H334" s="9"/>
       <c r="J334" s="9"/>
     </row>
-    <row r="335" spans="7:10" ht="18.75" customHeight="1">
+    <row r="335" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G335" s="9"/>
       <c r="H335" s="9"/>
       <c r="J335" s="9"/>
     </row>
-    <row r="336" spans="7:10" ht="18.75" customHeight="1">
+    <row r="336" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G336" s="9"/>
       <c r="H336" s="9"/>
       <c r="J336" s="9"/>
     </row>
-    <row r="337" spans="7:10" ht="18.75" customHeight="1">
+    <row r="337" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G337" s="9"/>
       <c r="H337" s="9"/>
       <c r="J337" s="9"/>
     </row>
-    <row r="338" spans="7:10" ht="18.75" customHeight="1">
+    <row r="338" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G338" s="9"/>
       <c r="H338" s="9"/>
       <c r="J338" s="9"/>
     </row>
-    <row r="339" spans="7:10" ht="18.75" customHeight="1">
+    <row r="339" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G339" s="9"/>
       <c r="H339" s="9"/>
       <c r="J339" s="9"/>
     </row>
-    <row r="340" spans="7:10" ht="18.75" customHeight="1">
+    <row r="340" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G340" s="9"/>
       <c r="H340" s="9"/>
       <c r="J340" s="9"/>
     </row>
-    <row r="341" spans="7:10" ht="18.75" customHeight="1">
+    <row r="341" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G341" s="9"/>
       <c r="H341" s="9"/>
       <c r="J341" s="9"/>
     </row>
-    <row r="342" spans="7:10" ht="18.75" customHeight="1">
+    <row r="342" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G342" s="9"/>
       <c r="H342" s="9"/>
       <c r="J342" s="9"/>
     </row>
-    <row r="343" spans="7:10" ht="18.75" customHeight="1">
+    <row r="343" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G343" s="9"/>
       <c r="H343" s="9"/>
       <c r="J343" s="9"/>
     </row>
-    <row r="344" spans="7:10" ht="18.75" customHeight="1">
+    <row r="344" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G344" s="9"/>
       <c r="H344" s="9"/>
       <c r="J344" s="9"/>
     </row>
-    <row r="345" spans="7:10" ht="18.75" customHeight="1">
+    <row r="345" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G345" s="9"/>
       <c r="H345" s="9"/>
       <c r="J345" s="9"/>
     </row>
-    <row r="346" spans="7:10" ht="18.75" customHeight="1">
+    <row r="346" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G346" s="9"/>
       <c r="H346" s="9"/>
       <c r="J346" s="9"/>
     </row>
-    <row r="347" spans="7:10" ht="18.75" customHeight="1">
+    <row r="347" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G347" s="9"/>
       <c r="H347" s="9"/>
       <c r="J347" s="9"/>
     </row>
-    <row r="348" spans="7:10" ht="18.75" customHeight="1">
+    <row r="348" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G348" s="9"/>
       <c r="H348" s="9"/>
       <c r="J348" s="9"/>
     </row>
-    <row r="349" spans="7:10" ht="18.75" customHeight="1">
+    <row r="349" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G349" s="9"/>
       <c r="H349" s="9"/>
       <c r="J349" s="9"/>
     </row>
-    <row r="350" spans="7:10" ht="18.75" customHeight="1">
+    <row r="350" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G350" s="9"/>
       <c r="H350" s="9"/>
       <c r="J350" s="9"/>
     </row>
-    <row r="351" spans="7:10" ht="18.75" customHeight="1">
+    <row r="351" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G351" s="9"/>
       <c r="H351" s="9"/>
       <c r="J351" s="9"/>
     </row>
-    <row r="352" spans="7:10" ht="18.75" customHeight="1">
+    <row r="352" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G352" s="9"/>
       <c r="H352" s="9"/>
       <c r="J352" s="9"/>
     </row>
-    <row r="353" spans="7:10" ht="18.75" customHeight="1">
+    <row r="353" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G353" s="9"/>
       <c r="H353" s="9"/>
       <c r="J353" s="9"/>
     </row>
-    <row r="354" spans="7:10" ht="18.75" customHeight="1">
+    <row r="354" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G354" s="9"/>
       <c r="H354" s="9"/>
       <c r="J354" s="9"/>
     </row>
-    <row r="355" spans="7:10" ht="18.75" customHeight="1">
+    <row r="355" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G355" s="9"/>
       <c r="H355" s="9"/>
       <c r="J355" s="9"/>
     </row>
-    <row r="356" spans="7:10" ht="18.75" customHeight="1">
+    <row r="356" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G356" s="9"/>
       <c r="H356" s="9"/>
       <c r="J356" s="9"/>
     </row>
-    <row r="357" spans="7:10" ht="18.75" customHeight="1">
+    <row r="357" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G357" s="9"/>
       <c r="H357" s="9"/>
       <c r="J357" s="9"/>
     </row>
-    <row r="358" spans="7:10" ht="18.75" customHeight="1">
+    <row r="358" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G358" s="9"/>
       <c r="H358" s="9"/>
       <c r="J358" s="9"/>
     </row>
-    <row r="359" spans="7:10" ht="18.75" customHeight="1">
+    <row r="359" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G359" s="9"/>
       <c r="H359" s="9"/>
       <c r="J359" s="9"/>
     </row>
-    <row r="360" spans="7:10" ht="18.75" customHeight="1">
+    <row r="360" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G360" s="9"/>
       <c r="H360" s="9"/>
       <c r="J360" s="9"/>
     </row>
-    <row r="361" spans="7:10" ht="18.75" customHeight="1">
+    <row r="361" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G361" s="9"/>
       <c r="H361" s="9"/>
       <c r="J361" s="9"/>
     </row>
-    <row r="362" spans="7:10" ht="18.75" customHeight="1">
+    <row r="362" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G362" s="9"/>
       <c r="H362" s="9"/>
       <c r="J362" s="9"/>
     </row>
-    <row r="363" spans="7:10" ht="18.75" customHeight="1">
+    <row r="363" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G363" s="9"/>
       <c r="H363" s="9"/>
       <c r="J363" s="9"/>
     </row>
-    <row r="364" spans="7:10" ht="18.75" customHeight="1">
+    <row r="364" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G364" s="9"/>
       <c r="H364" s="9"/>
       <c r="J364" s="9"/>
     </row>
-    <row r="365" spans="7:10" ht="18.75" customHeight="1">
+    <row r="365" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G365" s="9"/>
       <c r="H365" s="9"/>
       <c r="J365" s="9"/>
     </row>
-    <row r="366" spans="7:10" ht="18.75" customHeight="1">
+    <row r="366" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G366" s="9"/>
       <c r="H366" s="9"/>
       <c r="J366" s="9"/>
     </row>
-    <row r="367" spans="7:10" ht="18.75" customHeight="1">
+    <row r="367" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G367" s="9"/>
       <c r="H367" s="9"/>
       <c r="J367" s="9"/>
     </row>
-    <row r="368" spans="7:10" ht="18.75" customHeight="1">
+    <row r="368" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G368" s="9"/>
       <c r="H368" s="9"/>
       <c r="J368" s="9"/>
     </row>
-    <row r="369" spans="7:10" ht="18.75" customHeight="1">
+    <row r="369" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G369" s="9"/>
       <c r="H369" s="9"/>
       <c r="J369" s="9"/>
     </row>
-    <row r="370" spans="7:10" ht="18.75" customHeight="1">
+    <row r="370" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G370" s="9"/>
       <c r="H370" s="9"/>
       <c r="J370" s="9"/>
     </row>
-    <row r="371" spans="7:10" ht="18.75" customHeight="1">
+    <row r="371" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G371" s="9"/>
       <c r="H371" s="9"/>
       <c r="J371" s="9"/>
     </row>
-    <row r="372" spans="7:10" ht="18.75" customHeight="1">
+    <row r="372" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G372" s="9"/>
       <c r="H372" s="9"/>
       <c r="J372" s="9"/>
     </row>
-    <row r="373" spans="7:10" ht="18.75" customHeight="1">
+    <row r="373" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G373" s="9"/>
       <c r="H373" s="9"/>
       <c r="J373" s="9"/>
     </row>
-    <row r="374" spans="7:10" ht="18.75" customHeight="1">
+    <row r="374" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G374" s="9"/>
       <c r="H374" s="9"/>
       <c r="J374" s="9"/>
     </row>
-    <row r="375" spans="7:10" ht="18.75" customHeight="1">
+    <row r="375" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G375" s="9"/>
       <c r="H375" s="9"/>
       <c r="J375" s="9"/>
     </row>
-    <row r="376" spans="7:10" ht="18.75" customHeight="1">
+    <row r="376" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G376" s="9"/>
       <c r="H376" s="9"/>
       <c r="J376" s="9"/>
     </row>
-    <row r="377" spans="7:10" ht="18.75" customHeight="1">
+    <row r="377" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G377" s="9"/>
       <c r="H377" s="9"/>
       <c r="J377" s="9"/>
     </row>
-    <row r="378" spans="7:10" ht="18.75" customHeight="1">
+    <row r="378" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G378" s="9"/>
       <c r="H378" s="9"/>
       <c r="J378" s="9"/>
     </row>
-    <row r="379" spans="7:10" ht="18.75" customHeight="1">
+    <row r="379" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G379" s="9"/>
       <c r="H379" s="9"/>
       <c r="J379" s="9"/>
     </row>
-    <row r="380" spans="7:10" ht="18.75" customHeight="1">
+    <row r="380" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G380" s="9"/>
       <c r="H380" s="9"/>
       <c r="J380" s="9"/>
     </row>
-    <row r="381" spans="7:10" ht="18.75" customHeight="1">
+    <row r="381" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G381" s="9"/>
       <c r="J381" s="9"/>
     </row>
-    <row r="382" spans="7:10" ht="18.75" customHeight="1">
+    <row r="382" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G382" s="9"/>
     </row>
-    <row r="383" spans="7:10" ht="18.75" customHeight="1">
+    <row r="383" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G383" s="9"/>
     </row>
-    <row r="384" spans="7:10" ht="18.75" customHeight="1">
+    <row r="384" spans="7:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G384" s="9"/>
     </row>
-    <row r="385" spans="7:7" ht="18.75" customHeight="1">
+    <row r="385" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G385" s="9"/>
     </row>
-    <row r="386" spans="7:7" ht="18.75" customHeight="1">
+    <row r="386" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G386" s="9"/>
     </row>
-    <row r="387" spans="7:7" ht="18.75" customHeight="1">
+    <row r="387" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G387" s="9"/>
     </row>
-    <row r="388" spans="7:7" ht="18.75" customHeight="1">
+    <row r="388" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G388" s="9"/>
     </row>
-    <row r="389" spans="7:7" ht="18.75" customHeight="1">
+    <row r="389" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G389" s="9"/>
     </row>
-    <row r="390" spans="7:7" ht="18.75" customHeight="1">
+    <row r="390" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G390" s="9"/>
     </row>
-    <row r="391" spans="7:7" ht="18.75" customHeight="1">
+    <row r="391" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G391" s="9"/>
     </row>
-    <row r="392" spans="7:7" ht="18.75" customHeight="1">
+    <row r="392" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G392" s="9"/>
     </row>
-    <row r="393" spans="7:7" ht="18.75" customHeight="1">
+    <row r="393" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G393" s="9"/>
     </row>
-    <row r="394" spans="7:7" ht="18.75" customHeight="1">
+    <row r="394" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G394" s="9"/>
     </row>
-    <row r="395" spans="7:7" ht="18.75" customHeight="1">
+    <row r="395" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G395" s="9"/>
     </row>
-    <row r="396" spans="7:7" ht="18.75" customHeight="1">
+    <row r="396" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G396" s="9"/>
     </row>
-    <row r="397" spans="7:7" ht="18.75" customHeight="1">
+    <row r="397" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G397" s="9"/>
     </row>
-    <row r="398" spans="7:7" ht="18.75" customHeight="1">
+    <row r="398" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G398" s="9"/>
     </row>
-    <row r="399" spans="7:7" ht="18.75" customHeight="1">
+    <row r="399" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G399" s="9"/>
     </row>
   </sheetData>
@@ -5616,13 +5426,13 @@
     <sortCondition ref="BE16"/>
   </sortState>
   <conditionalFormatting sqref="B5:J1048576">
-    <cfRule type="expression" dxfId="32" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$J5="bestanden"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>OR($I5="ungenügend",$I5="mangelhaft")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$B5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5655,14 +5465,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J382" sqref="J382"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modultests Noten und News vom 23.08.
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben_Alle ( Axx )" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,16 @@
   </sheets>
   <definedNames>
     <definedName name="Auswahl">'Aufgaben_Alle ( Axx )'!$AJ$4:$AJ$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$65</definedName>
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="59">
   <si>
     <t>SWE Projekt HFTL-APP</t>
   </si>
@@ -380,28 +380,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -729,26 +708,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BE399"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="11" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="1.6640625" style="1" customWidth="1"/>
-    <col min="12" max="55" width="14.33203125" style="1"/>
-    <col min="56" max="56" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="14.33203125" style="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="11" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="1" customWidth="1"/>
+    <col min="12" max="55" width="14.28515625" style="1"/>
+    <col min="56" max="56" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="14.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="18.75" hidden="1" customHeight="1">
@@ -821,7 +800,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="28.8">
+    <row r="5" spans="1:57" ht="30">
       <c r="B5" s="16">
         <v>1</v>
       </c>
@@ -851,7 +830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="28.8">
+    <row r="6" spans="1:57" ht="30">
       <c r="B6" s="16">
         <f>IF(C6="","",B5+1)</f>
         <v>2</v>
@@ -882,7 +861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="28.8">
+    <row r="7" spans="1:57" ht="30">
       <c r="B7" s="16">
         <f t="shared" ref="B7:B72" si="0">IF(C7="","",B6+1)</f>
         <v>3</v>
@@ -913,7 +892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="28.8">
+    <row r="8" spans="1:57" ht="30">
       <c r="B8" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -949,7 +928,7 @@
       <c r="BD8" s="17"/>
       <c r="BE8" s="8"/>
     </row>
-    <row r="9" spans="1:57" ht="14.4">
+    <row r="9" spans="1:57" ht="15">
       <c r="B9" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1047,7 +1026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="14.4">
+    <row r="11" spans="1:57" ht="15">
       <c r="B11" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1139,7 +1118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="14.4">
+    <row r="13" spans="1:57" ht="15">
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1183,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="14.4">
+    <row r="14" spans="1:57" ht="15">
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1226,7 +1205,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="14.4">
+    <row r="15" spans="1:57" ht="15">
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1260,7 +1239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:57" ht="14.4">
+    <row r="16" spans="1:57" ht="15">
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1294,7 +1273,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="14.4">
+    <row r="17" spans="2:10" ht="15">
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1325,7 +1304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="14.4">
+    <row r="18" spans="2:10" ht="15">
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1443,7 +1422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="14.4">
+    <row r="22" spans="2:10" ht="15">
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2566,30 +2545,66 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B60" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
+      <c r="B60" s="16">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C60" s="9">
+        <v>42239</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="I60" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J60" s="9"/>
+        <v>befriedigend</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="61" spans="2:10" ht="18.75" customHeight="1">
-      <c r="B61" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
+      <c r="B61" s="16">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C61" s="9">
+        <v>42239</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="I61" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J61" s="9"/>
+        <v>sehr gut</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="62" spans="2:10" ht="18.75" customHeight="1">
       <c r="B62" s="16" t="str">
@@ -5484,13 +5499,13 @@
     <sortCondition ref="BE16"/>
   </sortState>
   <conditionalFormatting sqref="B5:J1048576">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$J5="bestanden"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>OR($I5="ungenügend",$I5="mangelhaft")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$B5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5530,7 +5545,7 @@
       <selection activeCell="J382" sqref="J382"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hoffentlich letzter Bugfix Doku 1.0
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/00_Testübersicht.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="Auswahl">'Aufgaben_Alle ( Axx )'!$AJ$4:$AJ$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$70</definedName>
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
@@ -714,7 +714,7 @@
   <dimension ref="A1:BE399"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>

</xml_diff>